<commit_message>
asset tracking updates and restructure
</commit_message>
<xml_diff>
--- a/ion/services/sa/observatory/test_xls/test505-a.xlsx
+++ b/ion/services/sa/observatory/test_xls/test505-a.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="6380" windowWidth="25600" windowHeight="13820" tabRatio="848" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="848" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CodeSpaces" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="247">
   <si>
     <t>CodeSpace ID</t>
   </si>
@@ -730,13 +730,49 @@
   </si>
   <si>
     <t>RTM-RAN-43</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>indigo</t>
+  </si>
+  <si>
+    <t>violet</t>
+  </si>
+  <si>
+    <t>pink</t>
+  </si>
+  <si>
+    <t>This is the color pink.</t>
+  </si>
+  <si>
+    <t>colors</t>
+  </si>
+  <si>
+    <t>Valid colors for testing</t>
+  </si>
+  <si>
+    <t>red, orange, yellow, green, blue, indigo, violet, pink</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -782,6 +818,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Verdana"/>
     </font>
   </fonts>
@@ -1428,7 +1470,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1552,8 +1594,20 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1816,8 +1870,20 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="41">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1858,6 +1924,10 @@
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2313,10 +2383,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IU107"/>
+  <dimension ref="A1:IU115"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView showGridLines="0" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="C110" sqref="C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
@@ -3634,6 +3704,118 @@
       </c>
       <c r="D107" s="2" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="18" customHeight="1">
+      <c r="A108" s="70" t="s">
+        <v>219</v>
+      </c>
+      <c r="B108" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C108" s="104" t="s">
+        <v>235</v>
+      </c>
+      <c r="D108" s="104" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="18" customHeight="1">
+      <c r="A109" s="70" t="s">
+        <v>219</v>
+      </c>
+      <c r="B109" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C109" s="104" t="s">
+        <v>236</v>
+      </c>
+      <c r="D109" s="104" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="18" customHeight="1">
+      <c r="A110" s="70" t="s">
+        <v>219</v>
+      </c>
+      <c r="B110" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C110" s="104" t="s">
+        <v>237</v>
+      </c>
+      <c r="D110" s="104" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="18" customHeight="1">
+      <c r="A111" s="70" t="s">
+        <v>219</v>
+      </c>
+      <c r="B111" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C111" s="104" t="s">
+        <v>238</v>
+      </c>
+      <c r="D111" s="104" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="18" customHeight="1">
+      <c r="A112" s="70" t="s">
+        <v>219</v>
+      </c>
+      <c r="B112" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C112" s="104" t="s">
+        <v>239</v>
+      </c>
+      <c r="D112" s="104" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="18" customHeight="1">
+      <c r="A113" s="70" t="s">
+        <v>219</v>
+      </c>
+      <c r="B113" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C113" s="104" t="s">
+        <v>240</v>
+      </c>
+      <c r="D113" s="104" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="18" customHeight="1">
+      <c r="A114" s="70" t="s">
+        <v>219</v>
+      </c>
+      <c r="B114" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C114" s="104" t="s">
+        <v>241</v>
+      </c>
+      <c r="D114" s="104" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="18" customHeight="1">
+      <c r="A115" s="70" t="s">
+        <v>219</v>
+      </c>
+      <c r="B115" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C115" s="104" t="s">
+        <v>242</v>
+      </c>
+      <c r="D115" s="104" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -3655,10 +3837,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IV13"/>
+  <dimension ref="A1:IV14"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A13" sqref="A2:A13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
@@ -3890,6 +4072,23 @@
       </c>
       <c r="E13" s="19" t="s">
         <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="18" customHeight="1">
+      <c r="A14" s="70" t="s">
+        <v>219</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="105" t="s">
+        <v>244</v>
+      </c>
+      <c r="D14" s="106" t="s">
+        <v>245</v>
+      </c>
+      <c r="E14" s="107" t="s">
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -4616,7 +4815,7 @@
   </sheetPr>
   <dimension ref="A1:IV2"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>

</xml_diff>